<commit_message>
vou comecar a usar o tensorflow
</commit_message>
<xml_diff>
--- a/Experimentos rubelmar/2018 Cruz Neto Polar wide.xlsx
+++ b/Experimentos rubelmar/2018 Cruz Neto Polar wide.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9388fc285210165e/_DOCÊNCIA/UEA/ALUNOS/2025c_Paper_Caio Dias/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thiag\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{C782ECA6-1859-4336-8E21-0F89C4C60C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA459A52-EA7F-4A19-90C5-C335FB8AEA20}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEC4455-C7FD-4A55-B945-30B65931D759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{62009AAF-A32E-435B-B345-387472B92711}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{62009AAF-A32E-435B-B345-387472B92711}"/>
   </bookViews>
   <sheets>
     <sheet name="Geometry-Dataset" sheetId="3" r:id="rId1"/>
@@ -24,9 +24,10 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -167,9 +168,6 @@
     <t>2C-09</t>
   </si>
   <si>
-    <t>2C -10</t>
-  </si>
-  <si>
     <t>2C-11</t>
   </si>
   <si>
@@ -192,6 +190,9 @@
   </si>
   <si>
     <t>Thickness (mm)</t>
+  </si>
+  <si>
+    <t>2C-10</t>
   </si>
 </sst>
 </file>
@@ -783,9 +784,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -823,7 +824,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -929,7 +930,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1071,7 +1072,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1081,18 +1082,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECEDC77B-DA06-4933-8815-006D833EF650}">
   <dimension ref="A1:NB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="MI1" workbookViewId="0">
-      <selection activeCell="MX15" sqref="MX15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -1100,13 +1101,13 @@
         <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="F1" s="1">
         <v>0</v>
@@ -2192,7 +2193,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="2" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3292,7 +3293,7 @@
         <v>4.2116402116402121</v>
       </c>
     </row>
-    <row r="3" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -4392,7 +4393,7 @@
         <v>3.8095238095238089</v>
       </c>
     </row>
-    <row r="4" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -5492,7 +5493,7 @@
         <v>3.9153439153439149</v>
       </c>
     </row>
-    <row r="5" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -6592,7 +6593,7 @@
         <v>4.0211640211640196</v>
       </c>
     </row>
-    <row r="6" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -7692,7 +7693,7 @@
         <v>4.35978835978836</v>
       </c>
     </row>
-    <row r="7" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -8792,7 +8793,7 @@
         <v>4.6560846560846558</v>
       </c>
     </row>
-    <row r="8" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -9892,7 +9893,7 @@
         <v>4.0846560846560847</v>
       </c>
     </row>
-    <row r="9" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -10992,7 +10993,7 @@
         <v>3.661375661375661</v>
       </c>
     </row>
-    <row r="10" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -12092,7 +12093,7 @@
         <v>3.0052910052910051</v>
       </c>
     </row>
-    <row r="11" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -13192,7 +13193,7 @@
         <v>3.4285714285714279</v>
       </c>
     </row>
-    <row r="12" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -14292,7 +14293,7 @@
         <v>4.4444444444444438</v>
       </c>
     </row>
-    <row r="13" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -15392,7 +15393,7 @@
         <v>2.941798941798941</v>
       </c>
     </row>
-    <row r="14" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -16492,7 +16493,7 @@
         <v>4.0423280423280419</v>
       </c>
     </row>
-    <row r="15" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -17592,7 +17593,7 @@
         <v>3.3227513227513228</v>
       </c>
     </row>
-    <row r="16" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -18692,7 +18693,7 @@
         <v>4.5291005291005284</v>
       </c>
     </row>
-    <row r="17" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -19792,7 +19793,7 @@
         <v>3.153439153439153</v>
       </c>
     </row>
-    <row r="18" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -20892,7 +20893,7 @@
         <v>4.2751322751322753</v>
       </c>
     </row>
-    <row r="19" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -21992,12 +21993,12 @@
         <v>4.2328042328042326</v>
       </c>
     </row>
-    <row r="20" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2">
         <v>3.577</v>
@@ -23092,12 +23093,12 @@
         <v>3.5767195767195772</v>
       </c>
     </row>
-    <row r="21" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C21" s="2">
         <v>3.5840000000000001</v>
@@ -24192,12 +24193,12 @@
         <v>4.1481481481481479</v>
       </c>
     </row>
-    <row r="22" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="2">
         <v>3.5720000000000001</v>
@@ -25292,12 +25293,12 @@
         <v>3.5978835978835981</v>
       </c>
     </row>
-    <row r="23" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="2">
         <v>3.4750000000000001</v>
@@ -26392,12 +26393,12 @@
         <v>3.8306878306878311</v>
       </c>
     </row>
-    <row r="24" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2">
         <v>3.4660000000000002</v>
@@ -27492,12 +27493,12 @@
         <v>3.9153439153439149</v>
       </c>
     </row>
-    <row r="25" spans="1:366" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:366" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C25" s="2">
         <v>3.444</v>

</xml_diff>